<commit_message>
new expenses, reorg of folders
</commit_message>
<xml_diff>
--- a/expenses/expenses.xlsx
+++ b/expenses/expenses.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>date</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>TOTAL</t>
+  </si>
+  <si>
+    <t>Resistors, rotary encoder, buttons</t>
   </si>
 </sst>
 </file>
@@ -177,12 +180,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="19">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -535,7 +538,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -546,17 +549,17 @@
     <col min="4" max="4" width="17.6640625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="5" customFormat="1" ht="43" customHeight="1" thickBot="1">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:4" s="4" customFormat="1" ht="43" customHeight="1" thickBot="1">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -644,14 +647,28 @@
         <v>90.24</v>
       </c>
     </row>
-    <row r="21" spans="2:4" s="4" customFormat="1" ht="38" customHeight="1" thickBot="1">
-      <c r="B21" s="3" t="s">
+    <row r="8" spans="1:4">
+      <c r="A8" s="1">
+        <v>42459</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="2">
+        <v>49.35</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" s="3" customFormat="1" ht="38" customHeight="1" thickBot="1">
+      <c r="B21" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="4">
+      <c r="C21" s="6"/>
+      <c r="D21" s="3">
         <f>SUM(D2:D20)</f>
-        <v>239.19</v>
+        <v>288.54000000000002</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="16" thickTop="1"/>

</xml_diff>